<commit_message>
added figures for a 75 mm wheel
</commit_message>
<xml_diff>
--- a/TimeBetweenSlots.xlsx
+++ b/TimeBetweenSlots.xlsx
@@ -37,6 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,7 +71,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,255 +373,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O8"/>
+  <dimension ref="B1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G1" t="s">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
+        <v>75</v>
+      </c>
+      <c r="E4">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>200</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>250</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>300</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>350</v>
       </c>
-      <c r="K4">
+      <c r="L4">
+        <v>75</v>
+      </c>
+      <c r="M4">
         <v>100</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>200</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>250</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>300</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" s="1">
         <f>1/(($C$5/3600*1000*1000)/(D4*3.414))/100*1000</f>
+        <v>1.8435600000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>1/(($C$5/3600*1000*1000)/(E4*3.414))/100*1000</f>
         <v>2.4580800000000003</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" ref="E5:H5" si="0">1/(($C$5/3600*1000*1000)/(E4*3.414))/100*1000</f>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:I5" si="0">1/(($C$5/3600*1000*1000)/(F4*3.414))/100*1000</f>
         <v>4.9161600000000005</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>6.1452000000000009</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>7.3742400000000004</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>8.6032799999999998</v>
       </c>
-      <c r="J5">
+      <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="K5" s="1">
-        <f>1/(($C$5/3600*1000*1000)/(K4*3.414))/8*1000</f>
+      <c r="L5" s="1">
+        <f>1/(($C$5/3600*1000*1000)/(L4*3.414))/8*1000</f>
+        <v>23.044500000000003</v>
+      </c>
+      <c r="M5" s="1">
+        <f>1/(($C$5/3600*1000*1000)/(M4*3.414))/8*1000</f>
         <v>30.726000000000003</v>
       </c>
-      <c r="L5" s="1">
-        <f t="shared" ref="L5:O5" si="1">1/(($C$5/3600*1000*1000)/(L4*3.414))/8*1000</f>
+      <c r="N5" s="1">
+        <f t="shared" ref="N5:Q5" si="1">1/(($C$5/3600*1000*1000)/(N4*3.414))/8*1000</f>
         <v>61.452000000000005</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <f t="shared" si="1"/>
         <v>76.815000000000012</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" s="1">
         <f t="shared" si="1"/>
         <v>92.178000000000011</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <f t="shared" si="1"/>
         <v>107.541</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" s="1">
         <f>1/(($C$6/3600*1000*1000)/(D4*3.414))/100*1000</f>
+        <v>0.92178000000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <f>1/(($C$6/3600*1000*1000)/(E4*3.414))/100*1000</f>
         <v>1.2290400000000001</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" ref="E6:H6" si="2">1/(($C$6/3600*1000*1000)/(E4*3.414))/100*1000</f>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:I6" si="2">1/(($C$6/3600*1000*1000)/(F4*3.414))/100*1000</f>
         <v>2.4580800000000003</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <f t="shared" si="2"/>
         <v>3.0726000000000004</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="2"/>
         <v>3.6871200000000002</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="2"/>
         <v>4.3016399999999999</v>
       </c>
-      <c r="J6">
+      <c r="K6" s="1">
         <v>10</v>
       </c>
-      <c r="K6" s="1">
-        <f>1/(($C$6/3600*1000*1000)/(K4*3.414))/8*1000</f>
+      <c r="L6" s="1">
+        <f>1/(($C$6/3600*1000*1000)/(L4*3.414))/8*1000</f>
+        <v>11.522250000000001</v>
+      </c>
+      <c r="M6" s="1">
+        <f>1/(($C$6/3600*1000*1000)/(M4*3.414))/8*1000</f>
         <v>15.363000000000001</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" ref="L6:O6" si="3">1/(($C$6/3600*1000*1000)/(L4*3.414))/8*1000</f>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:Q6" si="3">1/(($C$6/3600*1000*1000)/(N4*3.414))/8*1000</f>
         <v>30.726000000000003</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <f t="shared" si="3"/>
         <v>38.407500000000006</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <f t="shared" si="3"/>
         <v>46.089000000000006</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <f t="shared" si="3"/>
         <v>53.770499999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" s="1">
         <f>1/(($C$7/3600*1000*1000)/(D4*3.414))/100*1000</f>
+        <v>0.61452000000000007</v>
+      </c>
+      <c r="E7" s="1">
+        <f>1/(($C$7/3600*1000*1000)/(E4*3.414))/100*1000</f>
         <v>0.81935999999999998</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" ref="E7:H7" si="4">1/(($C$7/3600*1000*1000)/(E4*3.414))/100*1000</f>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:I7" si="4">1/(($C$7/3600*1000*1000)/(F4*3.414))/100*1000</f>
         <v>1.63872</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <f t="shared" si="4"/>
         <v>2.0484</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="4"/>
         <v>2.4580800000000003</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <f t="shared" si="4"/>
         <v>2.8677600000000005</v>
       </c>
-      <c r="J7">
+      <c r="K7" s="1">
         <v>15</v>
       </c>
-      <c r="K7" s="1">
-        <f>1/(($C$7/3600*1000*1000)/(K4*3.414))/8*1000</f>
+      <c r="L7" s="1">
+        <f>1/(($C$7/3600*1000*1000)/(L4*3.414))/8*1000</f>
+        <v>7.6815000000000007</v>
+      </c>
+      <c r="M7" s="1">
+        <f>1/(($C$7/3600*1000*1000)/(M4*3.414))/8*1000</f>
         <v>10.241999999999999</v>
       </c>
-      <c r="L7" s="1">
-        <f t="shared" ref="L7:O7" si="5">1/(($C$7/3600*1000*1000)/(L4*3.414))/8*1000</f>
+      <c r="N7" s="1">
+        <f t="shared" ref="N7:Q7" si="5">1/(($C$7/3600*1000*1000)/(N4*3.414))/8*1000</f>
         <v>20.483999999999998</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <f t="shared" si="5"/>
         <v>25.605</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <f t="shared" si="5"/>
         <v>30.726000000000003</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <f t="shared" si="5"/>
         <v>35.847000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>20</v>
       </c>
       <c r="D8" s="1">
         <f>1/(($C$8/3600*1000*1000)/(D4*3.414))/100*1000</f>
+        <v>0.46089000000000002</v>
+      </c>
+      <c r="E8" s="1">
+        <f>1/(($C$8/3600*1000*1000)/(E4*3.414))/100*1000</f>
         <v>0.61452000000000007</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" ref="E8:H8" si="6">1/(($C$8/3600*1000*1000)/(E4*3.414))/100*1000</f>
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:I8" si="6">1/(($C$8/3600*1000*1000)/(F4*3.414))/100*1000</f>
         <v>1.2290400000000001</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <f t="shared" si="6"/>
         <v>1.5363000000000002</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="6"/>
         <v>1.8435600000000001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <f t="shared" si="6"/>
         <v>2.15082</v>
       </c>
-      <c r="J8">
+      <c r="K8" s="1">
         <v>20</v>
       </c>
-      <c r="K8" s="1">
-        <f>1/(($C$8/3600*1000*1000)/(K4*3.414))/8*1000</f>
+      <c r="L8" s="1">
+        <f>1/(($C$8/3600*1000*1000)/(L4*3.414))/8*1000</f>
+        <v>5.7611250000000007</v>
+      </c>
+      <c r="M8" s="1">
+        <f>1/(($C$8/3600*1000*1000)/(M4*3.414))/8*1000</f>
         <v>7.6815000000000007</v>
       </c>
-      <c r="L8" s="1">
-        <f t="shared" ref="L8:O8" si="7">1/(($C$8/3600*1000*1000)/(L4*3.414))/8*1000</f>
+      <c r="N8" s="1">
+        <f t="shared" ref="N8:Q8" si="7">1/(($C$8/3600*1000*1000)/(N4*3.414))/8*1000</f>
         <v>15.363000000000001</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O8" s="1">
         <f t="shared" si="7"/>
         <v>19.203750000000003</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="1">
         <f t="shared" si="7"/>
         <v>23.044500000000003</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <f t="shared" si="7"/>
         <v>26.885249999999999</v>
       </c>

</xml_diff>